<commit_message>
before delete the comparison with LLA
</commit_message>
<xml_diff>
--- a/figures/Ericsson.xlsx
+++ b/figures/Ericsson.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="19440" windowHeight="12240"/>
@@ -105,26 +105,26 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -156,10 +156,78 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -170,13 +238,25 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="zh-CN"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -198,6 +278,7 @@
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$2:$A$27</c:f>
@@ -393,6 +474,7 @@
               </a:srgbClr>
             </a:solidFill>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$2:$A$27</c:f>
@@ -498,16 +580,16 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>12</c:v>
@@ -519,7 +601,7 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>14</c:v>
@@ -540,7 +622,7 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>13</c:v>
@@ -567,15 +649,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="39817600"/>
-        <c:axId val="39819520"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="127867392"/>
+        <c:axId val="116119168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39817600"/>
+        <c:axId val="127867392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -601,7 +692,10 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -610,20 +704,22 @@
             <a:pPr>
               <a:defRPr lang="en-US"/>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39819520"/>
+        <c:crossAx val="116119168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39819520"/>
+        <c:axId val="116119168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:minorGridlines>
@@ -650,8 +746,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -660,10 +759,10 @@
             <a:pPr>
               <a:defRPr lang="en-US"/>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39817600"/>
+        <c:crossAx val="127867392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -680,6 +779,7 @@
           <c:h val="6.7018458919086102E-2"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:ln>
           <a:noFill/>
@@ -692,12 +792,13 @@
           <a:pPr>
             <a:defRPr lang="en-US" sz="1200"/>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -743,7 +844,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -817,6 +918,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -851,6 +953,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1026,12 +1129,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
@@ -1105,7 +1210,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2">
         <v>15</v>
@@ -1119,7 +1224,7 @@
         <v>27</v>
       </c>
       <c r="C7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7">
         <v>22</v>
@@ -1133,7 +1238,7 @@
         <v>33</v>
       </c>
       <c r="C8">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E8">
         <v>33</v>
@@ -1147,7 +1252,7 @@
         <v>21</v>
       </c>
       <c r="C9">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E9">
         <v>21</v>
@@ -1203,7 +1308,7 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E13" s="1">
         <v>16</v>
@@ -1300,8 +1405,8 @@
       <c r="B20">
         <v>17</v>
       </c>
-      <c r="C20">
-        <v>16</v>
+      <c r="C20" s="1">
+        <v>14</v>
       </c>
       <c r="E20" s="1">
         <v>17</v>
@@ -1414,12 +1519,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1427,12 +1532,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Comparison with LLA was deleted
</commit_message>
<xml_diff>
--- a/figures/Ericsson.xlsx
+++ b/figures/Ericsson.xlsx
@@ -160,74 +160,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -372,10 +304,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>18</c:v>
@@ -384,70 +316,70 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>25</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="20">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>18</c:v>
-                </c:pt>
                 <c:pt idx="25">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -568,82 +500,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="18">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="23">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="24">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>13</c:v>
-                </c:pt>
                 <c:pt idx="25">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -658,11 +590,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="127867392"/>
-        <c:axId val="116119168"/>
+        <c:axId val="148939264"/>
+        <c:axId val="156355968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="127867392"/>
+        <c:axId val="148939264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -707,7 +639,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="116119168"/>
+        <c:crossAx val="156355968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -715,7 +647,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116119168"/>
+        <c:axId val="156355968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -762,7 +694,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="127867392"/>
+        <c:crossAx val="148939264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1133,10 +1065,13 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
@@ -1151,13 +1086,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2">
-        <v>17</v>
-      </c>
-      <c r="E2">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1165,13 +1097,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3">
-        <v>12</v>
-      </c>
-      <c r="E3">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1182,11 +1111,9 @@
         <v>18</v>
       </c>
       <c r="C4">
-        <v>17</v>
-      </c>
-      <c r="E4">
-        <v>19</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
@@ -1196,108 +1123,91 @@
         <v>13</v>
       </c>
       <c r="C5">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>14</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1">
-        <v>14</v>
-      </c>
-      <c r="E6" s="2">
-        <v>15</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C7">
-        <v>21</v>
-      </c>
-      <c r="E7">
-        <v>22</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8">
-        <v>28</v>
-      </c>
-      <c r="E8">
-        <v>33</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9">
-        <v>19</v>
-      </c>
-      <c r="E9">
-        <v>21</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10">
-        <v>12</v>
-      </c>
-      <c r="E10">
-        <v>14</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11">
-        <v>18</v>
-      </c>
-      <c r="E11">
-        <v>20</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" s="1" customFormat="1">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1">
-        <v>25</v>
-      </c>
-      <c r="E12" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1308,207 +1218,177 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>14</v>
-      </c>
-      <c r="E13" s="1">
-        <v>16</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14">
-        <v>14</v>
-      </c>
-      <c r="E14" s="1">
-        <v>14</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15">
-        <v>24</v>
-      </c>
-      <c r="E15" s="1">
-        <v>25</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16">
-        <v>12</v>
-      </c>
-      <c r="E16" s="1">
-        <v>12</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17">
-        <v>12</v>
-      </c>
-      <c r="E17" s="1">
-        <v>12</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18">
-        <v>12</v>
-      </c>
-      <c r="E18" s="1">
-        <v>12</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19">
-        <v>13</v>
-      </c>
-      <c r="E19" s="1">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="1">
-        <v>14</v>
-      </c>
-      <c r="E20" s="1">
-        <v>17</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21">
-        <v>13</v>
-      </c>
-      <c r="E21" s="1">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22">
-        <v>23</v>
-      </c>
-      <c r="E22" s="1">
-        <v>29</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23">
-        <v>13</v>
-      </c>
-      <c r="E23" s="1">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24">
-        <v>18</v>
-      </c>
-      <c r="E24" s="1">
-        <v>24</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25">
-        <v>13</v>
-      </c>
-      <c r="E25" s="1">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26">
-        <v>13</v>
-      </c>
-      <c r="E26" s="1">
-        <v>18</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C27">
-        <v>12</v>
-      </c>
-      <c r="E27" s="1">
-        <v>12</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E27" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>